<commit_message>
Updated list of SMB2 items.
(lwio: r40133)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="18135" windowHeight="7905"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="18135" windowHeight="7905" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SRV (General)" sheetId="7" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="LSARPC" sheetId="4" r:id="rId5"/>
     <sheet name="SRVSVC" sheetId="5" r:id="rId6"/>
     <sheet name="NETLOGON" sheetId="6" r:id="rId7"/>
+    <sheet name="Apps-SMB-V1" sheetId="8" r:id="rId8"/>
+    <sheet name="Apps-SMB-V2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -78,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="283">
   <si>
     <t>API</t>
   </si>
@@ -668,46 +670,265 @@
     <t>SMB2/COM2_BREAK (0x12)</t>
   </si>
   <si>
-    <t>SMB2/Durable Handles</t>
-  </si>
-  <si>
-    <t>SMB2/COM2_NEGOTIATE/NTLM</t>
-  </si>
-  <si>
-    <t>Re-factor srv</t>
-  </si>
-  <si>
-    <t>Oplock/Async support</t>
-  </si>
-  <si>
-    <t>Support epoll transport</t>
-  </si>
-  <si>
-    <t>Support kqueue transport</t>
-  </si>
-  <si>
-    <t>Support interim messages for COM_TRANSACTION etc.</t>
-  </si>
-  <si>
-    <t>Support zero-copy</t>
-  </si>
-  <si>
-    <t>Support Metrics on Connections/Sessions/Trees/Files</t>
-  </si>
-  <si>
-    <t>Support Chaining (ANDX)</t>
-  </si>
-  <si>
-    <t>Support big-endian systems</t>
-  </si>
-  <si>
-    <t>SMB1/Resolve global tree id set (Data Domain)</t>
-  </si>
-  <si>
-    <t>SMB1/Support root fids (TreeConnect)</t>
-  </si>
-  <si>
-    <t>SMB1/Create default shares with appropriate security descriptors</t>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>MS-Word</t>
+  </si>
+  <si>
+    <t>MS-Excel</t>
+  </si>
+  <si>
+    <t>MS-Powerpoint</t>
+  </si>
+  <si>
+    <t>MS-Explorer</t>
+  </si>
+  <si>
+    <t>MS-Internet Explorer</t>
+  </si>
+  <si>
+    <t>Command Shell</t>
+  </si>
+  <si>
+    <t>Tortoise SVN (Checkouts)</t>
+  </si>
+  <si>
+    <t>Visio</t>
+  </si>
+  <si>
+    <t>MS-Project</t>
+  </si>
+  <si>
+    <t>Wireshark</t>
+  </si>
+  <si>
+    <t>Notepad</t>
+  </si>
+  <si>
+    <t>Outlook</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Safari</t>
+  </si>
+  <si>
+    <t>iTunes</t>
+  </si>
+  <si>
+    <t>Adobe Reader</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Openoffice</t>
+  </si>
+  <si>
+    <t>Quicktime</t>
+  </si>
+  <si>
+    <t>Software Install (MSI files)</t>
+  </si>
+  <si>
+    <t>Image previews/Thumbnails</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>SaveAs</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>epoll transport</t>
+  </si>
+  <si>
+    <t>kqueue transport</t>
+  </si>
+  <si>
+    <t>interim messages for COM_TRANSACTION etc.</t>
+  </si>
+  <si>
+    <t>zero-copy</t>
+  </si>
+  <si>
+    <t>Metrics on Connections/Sessions/Trees/Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> big-endian systems</t>
+  </si>
+  <si>
+    <t>Create default shares with appropriate security descriptors</t>
+  </si>
+  <si>
+    <t>SMB2-INFO-TYPE-FILE (0x01)</t>
+  </si>
+  <si>
+    <t>SMB2-INFO-TYPE-FILE-SYSTEM (0x02)</t>
+  </si>
+  <si>
+    <t>SMB2-INFO-TYPE-SECURITY (0x03)</t>
+  </si>
+  <si>
+    <t>SMB Info Level</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_INTERNAL (0x06)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_EA (0x07)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_BASIC (0x04)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_STANDARD (0x05)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_NETWORK_OPEN (0x22)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ACCESS (0x08)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_POSITION (0x0E)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_COMPRESSION (0x1C)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_FULL_EA (0x0F)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_STREAM (0x16)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ATTRIBUTE_TAG (0x23)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ALTERNATE_NAME (0x15)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ALIGNMENT (0x11)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ALL (0x12)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_MODE (0x10)</t>
+  </si>
+  <si>
+    <t>SMB2_FS_INFO_CLASS_VOLUME (0x01)</t>
+  </si>
+  <si>
+    <t>SMB2_FS_INFO_CLASS_ATTRIBUTE (0x05)</t>
+  </si>
+  <si>
+    <t>SMB2_FS_INFO_CLASS_FULL_SIZE (0x07)</t>
+  </si>
+  <si>
+    <t>SMB2_FS_INFO_CLASS_SIZE (0x03)</t>
+  </si>
+  <si>
+    <t>SMB_FS_INFO_CLASS_OBJECTID (0x08)</t>
+  </si>
+  <si>
+    <t>SMB2_FS_INFO_CLASS_DEVICE (0x04)</t>
+  </si>
+  <si>
+    <t>SMB2_FS_INFO_CLASS_QUOTA (0x06)</t>
+  </si>
+  <si>
+    <t>STATUS_NOT_SUPPORTED</t>
+  </si>
+  <si>
+    <t>SMB2_SEC_INFO_CLASS_BASIC</t>
+  </si>
+  <si>
+    <t>SMB2_SEC_INFO_CLASS_BASIC (0x00)</t>
+  </si>
+  <si>
+    <t>STATUS_SUCCESS</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_PIPE (0x17)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_EOF (0x14)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_DISPOSITION (0x0D)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_RENAME (0x0A)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ALLOCATION (0x13)</t>
+  </si>
+  <si>
+    <t>Kerberos</t>
+  </si>
+  <si>
+    <t>NTLM</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ID_BOTH_DIR (0x25)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_ID_FULL_DIR (0x26)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_BOTH_DIR (0x03)</t>
+  </si>
+  <si>
+    <t>SMB2_FILE_INFO_CLASS_FULL_DIR (0x04)</t>
+  </si>
+  <si>
+    <t>SMB2-INFO-TYPE-QUOTA (0x04)</t>
+  </si>
+  <si>
+    <t>Create Context (MxAC)</t>
+  </si>
+  <si>
+    <t>Create Context (DHnQ)</t>
+  </si>
+  <si>
+    <t>Query Disk Id</t>
+  </si>
+  <si>
+    <t>Maximal Access Mask</t>
+  </si>
+  <si>
+    <t>Durable Handle</t>
+  </si>
+  <si>
+    <t>Create Context (ExtA)</t>
+  </si>
+  <si>
+    <t>Create Context (Qfid)</t>
+  </si>
+  <si>
+    <t>Query Extended Attributes</t>
+  </si>
+  <si>
+    <t>Create Context (Twip)</t>
+  </si>
+  <si>
+    <t>Shadow Copy</t>
+  </si>
+  <si>
+    <t>Oplock Break</t>
+  </si>
+  <si>
+    <t>Needs re-visiting</t>
   </si>
 </sst>
 </file>
@@ -717,7 +938,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -752,6 +973,28 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -806,7 +1049,7 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -819,6 +1062,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Done" xfId="3"/>
@@ -1118,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1131,62 +1377,37 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1198,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A86" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -2156,144 +2377,575 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="D4" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="D5" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="D6" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="D7" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="D8" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>272</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E13" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="D14" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="D15" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="D16" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="D17" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="D18" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+      <c r="D19" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
+      <c r="D20" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="D21" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="C22" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" t="s">
+        <v>267</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" t="s">
+        <v>269</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="D26" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="B27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="C29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" t="s">
+        <v>234</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="C33" t="s">
+        <v>241</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="C34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="C35" t="s">
+        <v>245</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="C36" t="s">
+        <v>246</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="C37" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="C38" t="s">
+        <v>242</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="C39" t="s">
+        <v>240</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="C40" t="s">
+        <v>237</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="C41" t="s">
+        <v>243</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" t="s">
+        <v>230</v>
+      </c>
+      <c r="C42" t="s">
+        <v>248</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="C43" t="s">
+        <v>251</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="C44" t="s">
+        <v>253</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="C45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="C46" t="s">
+        <v>254</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="C47" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="C48" t="s">
+        <v>252</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="B49" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" t="s">
+        <v>257</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="B50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="B51" t="s">
+        <v>229</v>
+      </c>
+      <c r="C51" t="s">
+        <v>239</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="C52" t="s">
+        <v>247</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="C53" t="s">
+        <v>259</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="C54" t="s">
+        <v>260</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="C55" t="s">
+        <v>261</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="C56" t="s">
+        <v>262</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="C57" t="s">
+        <v>235</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="C58" t="s">
+        <v>263</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="B59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="B60" t="s">
+        <v>231</v>
+      </c>
+      <c r="C60" t="s">
+        <v>256</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" t="s">
+        <v>270</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>197</v>
+      <c r="D62" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E62" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4359,4 +5011,290 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="8" customFormat="1">
+      <c r="A1" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
indicate that SMB2_NOTIFY and SMB2_CANCEL are now implemented
(lwio: r40212)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -2380,7 +2380,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2581,8 +2581,8 @@
       <c r="A20" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>255</v>
+      <c r="D20" s="10" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2632,8 +2632,8 @@
       <c r="A26" t="s">
         <v>192</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>255</v>
+      <c r="D26" s="10" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:5">

</xml_diff>

<commit_message>
Check in updates to the SMB2 Application support matrix
(lwio: r40912)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="18135" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="18135" windowHeight="7905" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="SRV (General)" sheetId="7" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="NETLOGON" sheetId="6" r:id="rId7"/>
     <sheet name="Apps-SMB-V1" sheetId="8" r:id="rId8"/>
     <sheet name="Apps-SMB-V2" sheetId="9" r:id="rId9"/>
+    <sheet name="SMB2TORTURE" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="312">
   <si>
     <t>API</t>
   </si>
@@ -929,6 +930,93 @@
   </si>
   <si>
     <t>Needs re-visiting</t>
+  </si>
+  <si>
+    <t>SMB2-LOCK</t>
+  </si>
+  <si>
+    <t>SMB2-READ</t>
+  </si>
+  <si>
+    <t>SMB2-CREATE</t>
+  </si>
+  <si>
+    <t>SMB2-ACLS</t>
+  </si>
+  <si>
+    <t>SMB2-NOTIFY</t>
+  </si>
+  <si>
+    <t>SMB2-DURABLE-OPEN</t>
+  </si>
+  <si>
+    <t>SMB2-DIR</t>
+  </si>
+  <si>
+    <t>SMB2-LEASE</t>
+  </si>
+  <si>
+    <t>SMB2-COMPOUND</t>
+  </si>
+  <si>
+    <t>SMB2-OPLOCK</t>
+  </si>
+  <si>
+    <t>SMB2-STREAMS</t>
+  </si>
+  <si>
+    <t>SMB2-CONNECT</t>
+  </si>
+  <si>
+    <t>SMB2-SCAN</t>
+  </si>
+  <si>
+    <t>SMB2-GETINFO</t>
+  </si>
+  <si>
+    <t>SMB2-SCANGETINFO</t>
+  </si>
+  <si>
+    <t>SMB2-SCANSETINFO</t>
+  </si>
+  <si>
+    <t>SMB2-SCANFIND</t>
+  </si>
+  <si>
+    <t>SMB2-SETINFO</t>
+  </si>
+  <si>
+    <t>SMB2-HOLD-OPLOCK</t>
+  </si>
+  <si>
+    <t>SMB2-BENCH-OPLOCK</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Sub-test</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Later release</t>
+  </si>
+  <si>
+    <t>list directory</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>create directory</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1137,7 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1065,6 +1153,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Done" xfId="3"/>
@@ -1415,6 +1509,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="8" customFormat="1">
+      <c r="A1" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E123"/>
@@ -2379,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5160,141 +5395,378 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="7" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="12.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="E1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" s="11"/>
+      <c r="E2" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="E16" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="E17" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="E18" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="E19" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="E20" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="E21" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>217</v>
       </c>
+      <c r="E22" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>308</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update progress on testing some SMB2 application scenarios
(lwio: r41015)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="314">
   <si>
     <t>API</t>
   </si>
@@ -1004,19 +1004,25 @@
     <t>Later release</t>
   </si>
   <si>
-    <t>list directory</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>copy</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
-    <t>create directory</t>
+    <t>delete file</t>
+  </si>
+  <si>
+    <t>copy file</t>
+  </si>
+  <si>
+    <t>copy dir</t>
+  </si>
+  <si>
+    <t>delete dir</t>
+  </si>
+  <si>
+    <t>create dir</t>
+  </si>
+  <si>
+    <t>list dir</t>
   </si>
 </sst>
 </file>
@@ -5395,10 +5401,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5408,10 +5414,12 @@
     <col min="3" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="12.28515625" style="7" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="7" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1">
+    <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>196</v>
       </c>
@@ -5425,157 +5433,212 @@
         <v>220</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="12" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>197</v>
       </c>
       <c r="B2" s="11"/>
       <c r="E2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>198</v>
       </c>
+      <c r="B3" s="11"/>
       <c r="E3" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>199</v>
       </c>
+      <c r="B4" s="11"/>
       <c r="E4" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>200</v>
       </c>
+      <c r="B5" s="11"/>
       <c r="E5" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>201</v>
       </c>
+      <c r="B6" s="11"/>
       <c r="E6" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>202</v>
       </c>
+      <c r="B7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>203</v>
       </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>204</v>
       </c>
+      <c r="B9" s="11"/>
       <c r="E9" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>205</v>
       </c>
+      <c r="B10" s="11"/>
       <c r="E10" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>206</v>
       </c>
+      <c r="B11" s="11"/>
       <c r="E11" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -5583,186 +5646,260 @@
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>208</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>209</v>
       </c>
+      <c r="B14" s="11"/>
       <c r="E14" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>210</v>
       </c>
+      <c r="B15" s="11"/>
       <c r="E15" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>211</v>
       </c>
+      <c r="B16" s="11"/>
       <c r="E16" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>212</v>
       </c>
+      <c r="B17" s="11"/>
       <c r="E17" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>213</v>
       </c>
+      <c r="B18" s="11"/>
       <c r="E18" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>214</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>215</v>
       </c>
+      <c r="B20" s="11"/>
       <c r="E20" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>216</v>
       </c>
+      <c r="B21"/>
       <c r="E21" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>307</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>217</v>
       </c>
+      <c r="B22" s="11"/>
       <c r="E22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to SMB2 application matrix
(lwio: r41033)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="323">
   <si>
     <t>API</t>
   </si>
@@ -1023,6 +1023,33 @@
   </si>
   <si>
     <t>list dir</t>
+  </si>
+  <si>
+    <t>Works</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>W.I.P.</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>û</t>
+  </si>
+  <si>
+    <t>¡</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>MS-Word (doc format)</t>
+  </si>
+  <si>
+    <t>MS-Word (docx format)</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1059,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1090,8 +1117,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1116,6 +1168,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1135,15 +1192,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1159,16 +1217,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Done" xfId="3"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Neutral" xfId="6" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Partially Done" xfId="4"/>
     <cellStyle name="Pending" xfId="5"/>
@@ -5401,10 +5469,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5417,488 +5485,774 @@
     <col min="7" max="8" width="13.7109375" style="7" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" style="7" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="E2" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>307</v>
+        <v>321</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="E3" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>307</v>
+        <v>322</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="E4" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>307</v>
+        <v>198</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="E5" s="7" t="s">
-        <v>307</v>
+        <v>199</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="E6" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>307</v>
+        <v>200</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+        <v>201</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>204</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="E9" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>307</v>
+        <v>203</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="E10" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>307</v>
+        <v>204</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="E11" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>307</v>
+        <v>205</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>307</v>
+        <v>206</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>208</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>307</v>
+        <v>207</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="E14" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>307</v>
+        <v>208</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="E15" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>307</v>
+        <v>209</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>211</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="E16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>307</v>
+        <v>210</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="E17" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>307</v>
+        <v>211</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>213</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="E18" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>307</v>
+        <v>212</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>214</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>307</v>
+        <v>213</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>215</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="E20" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>307</v>
+        <v>214</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>216</v>
-      </c>
-      <c r="B21"/>
-      <c r="E21" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>307</v>
+        <v>215</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
         <v>217</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="E22" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="J22" s="7" t="s">
+      <c r="B23" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="B25" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="B26" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="B27" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>307</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to SMB2 Application support matrix
(lwio: r41075)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="324">
   <si>
     <t>API</t>
   </si>
@@ -1013,9 +1013,6 @@
     <t>copy file</t>
   </si>
   <si>
-    <t>copy dir</t>
-  </si>
-  <si>
     <t>delete dir</t>
   </si>
   <si>
@@ -1028,12 +1025,6 @@
     <t>Works</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>W.I.P.</t>
-  </si>
-  <si>
     <t>ü</t>
   </si>
   <si>
@@ -1050,6 +1041,18 @@
   </si>
   <si>
     <t>MS-Word (docx format)</t>
+  </si>
+  <si>
+    <t>T.B.D.</t>
+  </si>
+  <si>
+    <t>Fails</t>
+  </si>
+  <si>
+    <t>Drag/Drop</t>
+  </si>
+  <si>
+    <t>copy dir/xcopy</t>
   </si>
 </sst>
 </file>
@@ -5469,10 +5472,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5485,10 +5488,10 @@
     <col min="7" max="8" width="13.7109375" style="7" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" style="7" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="7" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1">
+    <row r="1" spans="1:11" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>196</v>
       </c>
@@ -5502,755 +5505,824 @@
         <v>220</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>309</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>308</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>310</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>318</v>
+        <v>314</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E2" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>319</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>322</v>
-      </c>
       <c r="B3" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>198</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>199</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>200</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>201</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>202</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>314</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>203</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>317</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>204</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>205</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>206</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>207</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>208</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>209</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>210</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>211</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>320</v>
-      </c>
       <c r="D17" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>212</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>320</v>
+      <c r="D18" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>213</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>320</v>
+        <v>314</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>214</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>320</v>
+      <c r="B20" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>215</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>320</v>
-      </c>
       <c r="D21" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>216</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>320</v>
+      <c r="B22" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>316</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>217</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="B25" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="B26" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C26" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="B25" s="12" t="s">
-        <v>317</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="B26" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:11">
       <c r="B27" s="13" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="B28" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>307</v>

</xml_diff>

<commit_message>
Update Application Matrix for SMB2
(lwio: r41103)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -5475,7 +5475,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5694,8 +5694,8 @@
       <c r="I6" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="J6" s="14" t="s">
-        <v>317</v>
+      <c r="J6" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>314</v>
@@ -5775,8 +5775,8 @@
       <c r="A9" t="s">
         <v>203</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>317</v>
+      <c r="B9" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>317</v>
@@ -6058,11 +6058,11 @@
       <c r="B17" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>317</v>
+      <c r="C17" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>316</v>

</xml_diff>

<commit_message>
Update SMB2 Application support matrix
(lwio: r41109)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -5475,7 +5475,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5950,14 +5950,14 @@
       <c r="A14" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>317</v>
+      <c r="B14" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>316</v>

</xml_diff>

<commit_message>
Updates to SMB2 Application Matrix. From Peter Chai.
(lwio: r41560)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -5475,7 +5475,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6198,11 +6198,11 @@
       <c r="B21" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>317</v>
+      <c r="C21" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>316</v>

</xml_diff>

<commit_message>
update smb2 application matrix
(lwio: r41572)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -5475,7 +5475,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5778,32 +5778,32 @@
       <c r="B9" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>317</v>
+      <c r="C9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:11">

</xml_diff>

<commit_message>
update smb2 torture status. update smb2 application matrix.
(lwio: r41633)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="18135" windowHeight="7905" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="18135" windowHeight="7905" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="SRV (General)" sheetId="7" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="324">
   <si>
     <t>API</t>
   </si>
@@ -1588,17 +1588,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1">
@@ -1619,31 +1620,49 @@
       <c r="A2" t="s">
         <v>285</v>
       </c>
+      <c r="C2" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>284</v>
       </c>
+      <c r="C3" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>283</v>
       </c>
+      <c r="C4" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>286</v>
       </c>
+      <c r="C5" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>287</v>
       </c>
+      <c r="C6" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>288</v>
       </c>
+      <c r="C7" s="14" t="s">
+        <v>317</v>
+      </c>
       <c r="D7" t="s">
         <v>306</v>
       </c>
@@ -1652,11 +1671,17 @@
       <c r="A8" t="s">
         <v>289</v>
       </c>
+      <c r="C8" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>290</v>
       </c>
+      <c r="C9" s="14" t="s">
+        <v>317</v>
+      </c>
       <c r="D9" t="s">
         <v>306</v>
       </c>
@@ -1665,60 +1690,128 @@
       <c r="A10" t="s">
         <v>291</v>
       </c>
+      <c r="C10" s="12" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>292</v>
       </c>
+      <c r="C11" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>293</v>
       </c>
+      <c r="C12" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>294</v>
       </c>
+      <c r="C13" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>295</v>
       </c>
+      <c r="C14" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>297</v>
       </c>
+      <c r="C15" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="C16" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C17" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="C19" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="C20" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>301</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -5474,8 +5567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6093,8 +6186,8 @@
       <c r="B18" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>317</v>
+      <c r="C18" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>314</v>

</xml_diff>

<commit_message>
Update SMB2 torture information
(lwio: r45012)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="443">
   <si>
     <t>API</t>
   </si>
@@ -1053,6 +1053,363 @@
   </si>
   <si>
     <t>copy dir/xcopy</t>
+  </si>
+  <si>
+    <t>Status/Windows</t>
+  </si>
+  <si>
+    <t>Status/Likewise</t>
+  </si>
+  <si>
+    <t>GENTEST</t>
+  </si>
+  <si>
+    <t>BLOB</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>BRLOCKED</t>
+  </si>
+  <si>
+    <t>MULTI</t>
+  </si>
+  <si>
+    <t>LEADING-SLASH</t>
+  </si>
+  <si>
+    <t>ACLFILE</t>
+  </si>
+  <si>
+    <t>ACLDIR</t>
+  </si>
+  <si>
+    <t>NULLDACL</t>
+  </si>
+  <si>
+    <t>EOF</t>
+  </si>
+  <si>
+    <t>POSITION</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>VALID-REQUEST</t>
+  </si>
+  <si>
+    <t>RW-NONE</t>
+  </si>
+  <si>
+    <t>RW-SHARED</t>
+  </si>
+  <si>
+    <t>RW-EXCLUSIVE</t>
+  </si>
+  <si>
+    <t>AUTO-UNLOCK</t>
+  </si>
+  <si>
+    <t>LOCK</t>
+  </si>
+  <si>
+    <t>ASYNC</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
+  </si>
+  <si>
+    <t>CANCEL-TDIS</t>
+  </si>
+  <si>
+    <t>CANCEL-LOGOFF</t>
+  </si>
+  <si>
+    <t>ERRORCODE</t>
+  </si>
+  <si>
+    <t>ZEROBYTELENGTH</t>
+  </si>
+  <si>
+    <t>ZEROBYTEREAD</t>
+  </si>
+  <si>
+    <t>UNLOCK</t>
+  </si>
+  <si>
+    <t>MULTIPLE-UNLOCK</t>
+  </si>
+  <si>
+    <t>STACKING</t>
+  </si>
+  <si>
+    <t>CONTEND</t>
+  </si>
+  <si>
+    <t>CONTEXT</t>
+  </si>
+  <si>
+    <t>RANGE</t>
+  </si>
+  <si>
+    <t>OVERLAP</t>
+  </si>
+  <si>
+    <t>TRUNCATE</t>
+  </si>
+  <si>
+    <t>CREATOR</t>
+  </si>
+  <si>
+    <t>GENERIC</t>
+  </si>
+  <si>
+    <t>OWNER</t>
+  </si>
+  <si>
+    <t>INHERITANCE</t>
+  </si>
+  <si>
+    <t>INHERITFLAGS</t>
+  </si>
+  <si>
+    <t>DYNAMIC</t>
+  </si>
+  <si>
+    <t>GETSET</t>
+  </si>
+  <si>
+    <t>VALID-REQ</t>
+  </si>
+  <si>
+    <t>TCON</t>
+  </si>
+  <si>
+    <t>MASK</t>
+  </si>
+  <si>
+    <t>TDIS</t>
+  </si>
+  <si>
+    <t>LOGOFF</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>MASK-CHANGE</t>
+  </si>
+  <si>
+    <t>TREE</t>
+  </si>
+  <si>
+    <t>BASEDIR</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>FILE</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t>OVERFLOW</t>
+  </si>
+  <si>
+    <t>FILE-POSITION</t>
+  </si>
+  <si>
+    <t>OPLOCK</t>
+  </si>
+  <si>
+    <t>LEASE</t>
+  </si>
+  <si>
+    <t>FIND</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>ONE</t>
+  </si>
+  <si>
+    <t>MANY</t>
+  </si>
+  <si>
+    <t>MODIFY</t>
+  </si>
+  <si>
+    <t>SORTED</t>
+  </si>
+  <si>
+    <t>FILE-INDEX</t>
+  </si>
+  <si>
+    <t>LARGE-FILES</t>
+  </si>
+  <si>
+    <t>REQUEST</t>
+  </si>
+  <si>
+    <t>UPGRADE</t>
+  </si>
+  <si>
+    <t>BREAK</t>
+  </si>
+  <si>
+    <t>MULTIBREAK</t>
+  </si>
+  <si>
+    <t>RELATED1</t>
+  </si>
+  <si>
+    <t>RELATED2</t>
+  </si>
+  <si>
+    <t>UNRELATED1</t>
+  </si>
+  <si>
+    <t>INVALID1</t>
+  </si>
+  <si>
+    <t>INVALID2</t>
+  </si>
+  <si>
+    <t>INVALID3</t>
+  </si>
+  <si>
+    <t>EXCLUSIVE1</t>
+  </si>
+  <si>
+    <t>EXCLUSIVE2</t>
+  </si>
+  <si>
+    <t>EXCLUSIVE3</t>
+  </si>
+  <si>
+    <t>EXCLUSIVE4</t>
+  </si>
+  <si>
+    <t>EXCLUSIVE5</t>
+  </si>
+  <si>
+    <t>EXCLUSIVE6</t>
+  </si>
+  <si>
+    <t>BATCH1</t>
+  </si>
+  <si>
+    <t>BATCH2</t>
+  </si>
+  <si>
+    <t>BATCH3</t>
+  </si>
+  <si>
+    <t>BATCH4</t>
+  </si>
+  <si>
+    <t>BATCH5</t>
+  </si>
+  <si>
+    <t>BATCH6</t>
+  </si>
+  <si>
+    <t>BATCH7</t>
+  </si>
+  <si>
+    <t>BATCH8</t>
+  </si>
+  <si>
+    <t>BATCH9</t>
+  </si>
+  <si>
+    <t>BATCH10</t>
+  </si>
+  <si>
+    <t>BATCH11</t>
+  </si>
+  <si>
+    <t>BATCH12</t>
+  </si>
+  <si>
+    <t>BATCH13</t>
+  </si>
+  <si>
+    <t>BATCH14</t>
+  </si>
+  <si>
+    <t>BATCH15</t>
+  </si>
+  <si>
+    <t>BATCH16</t>
+  </si>
+  <si>
+    <t>BATCH19</t>
+  </si>
+  <si>
+    <t>BATCH20</t>
+  </si>
+  <si>
+    <t>BATCH21</t>
+  </si>
+  <si>
+    <t>BATCH22</t>
+  </si>
+  <si>
+    <t>BATCH23</t>
+  </si>
+  <si>
+    <t>BATCH24</t>
+  </si>
+  <si>
+    <t>BATCH25</t>
+  </si>
+  <si>
+    <t>STREAM1</t>
+  </si>
+  <si>
+    <t>DOC</t>
+  </si>
+  <si>
+    <t>BRL1</t>
+  </si>
+  <si>
+    <t>BRL2</t>
+  </si>
+  <si>
+    <t>BRL3</t>
+  </si>
+  <si>
+    <t>LEVELII500</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>SHAREMODES</t>
+  </si>
+  <si>
+    <t>NAMES</t>
+  </si>
+  <si>
+    <t>NAMES2</t>
+  </si>
+  <si>
+    <t>RENAME2</t>
+  </si>
+  <si>
+    <t>CREATE-DISPOSITION</t>
+  </si>
+  <si>
+    <t>ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>lwiod does support file index</t>
   </si>
 </sst>
 </file>
@@ -1588,21 +1945,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1">
+    <row r="1" spans="1:5" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>303</v>
       </c>
@@ -1610,207 +1968,1585 @@
         <v>304</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>285</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>334</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>284</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="B12" t="s">
+        <v>335</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="B15" t="s">
+        <v>338</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>341</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>343</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>345</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" t="s">
+        <v>347</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>349</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>351</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>353</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>354</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" t="s">
+        <v>355</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="B33" t="s">
+        <v>356</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" t="s">
+        <v>357</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" t="s">
+        <v>358</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>286</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B36" t="s">
+        <v>359</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" t="s">
+        <v>360</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" t="s">
+        <v>361</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" t="s">
+        <v>362</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" t="s">
+        <v>363</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="B41" t="s">
+        <v>364</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="B42" t="s">
+        <v>365</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>287</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="B43" t="s">
+        <v>366</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" t="s">
+        <v>367</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="B45" t="s">
+        <v>337</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="B46" t="s">
+        <v>368</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" t="s">
+        <v>369</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="B48" t="s">
+        <v>370</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="B49" t="s">
+        <v>371</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="B50" t="s">
+        <v>372</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="B51" t="s">
+        <v>373</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="B52" t="s">
+        <v>374</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="B53" t="s">
+        <v>375</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="B54" t="s">
+        <v>376</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="B55" t="s">
+        <v>377</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="B56" t="s">
+        <v>378</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
         <v>288</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B57" t="s">
+        <v>379</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E57" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="58" spans="1:5">
+      <c r="B58" t="s">
+        <v>380</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E58" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="B59" t="s">
+        <v>381</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E59" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="B60" t="s">
+        <v>343</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E60" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" t="s">
+        <v>328</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E61" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="B62" t="s">
+        <v>382</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="B63" t="s">
+        <v>383</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="B64" t="s">
+        <v>384</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="B65" t="s">
+        <v>385</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="B66" t="s">
+        <v>386</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="B67" t="s">
+        <v>387</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="B68" t="s">
+        <v>388</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E68" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="B69" t="s">
+        <v>389</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
         <v>290</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B70" t="s">
+        <v>390</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E70" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="71" spans="1:5">
+      <c r="B71" t="s">
+        <v>391</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E71" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="B72" t="s">
+        <v>392</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E72" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="B73" t="s">
+        <v>380</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E73" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="B74" t="s">
+        <v>393</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E74" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
         <v>291</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="B75" t="s">
+        <v>394</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="B76" t="s">
+        <v>395</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="B77" t="s">
+        <v>396</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="B78" t="s">
+        <v>397</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="B79" t="s">
+        <v>398</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="B80" t="s">
+        <v>399</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
         <v>292</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="B81" t="s">
+        <v>400</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="B82" t="s">
+        <v>401</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="B83" t="s">
+        <v>402</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="B84" t="s">
+        <v>403</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="B85" t="s">
+        <v>404</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="B86" t="s">
+        <v>405</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="B87" t="s">
+        <v>406</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="B88" t="s">
+        <v>407</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="B89" t="s">
+        <v>408</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="B90" t="s">
+        <v>409</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="B91" t="s">
+        <v>410</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="B92" t="s">
+        <v>411</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="B93" t="s">
+        <v>412</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="B94" t="s">
+        <v>413</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="B95" t="s">
+        <v>414</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="B96" t="s">
+        <v>415</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" t="s">
+        <v>416</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" t="s">
+        <v>417</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4">
+      <c r="B99" t="s">
+        <v>418</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4">
+      <c r="B100" t="s">
+        <v>419</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4">
+      <c r="B101" t="s">
+        <v>420</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4">
+      <c r="B102" t="s">
+        <v>421</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4">
+      <c r="B103" t="s">
+        <v>422</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4">
+      <c r="B104" t="s">
+        <v>423</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4">
+      <c r="B105" t="s">
+        <v>424</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4">
+      <c r="B106" t="s">
+        <v>425</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4">
+      <c r="B107" t="s">
+        <v>426</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
+      <c r="B108" t="s">
+        <v>427</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4">
+      <c r="B109" t="s">
+        <v>428</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
+      <c r="B110" t="s">
+        <v>429</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
+      <c r="B111" t="s">
+        <v>430</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D111" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4">
+      <c r="B112" t="s">
+        <v>431</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="B113" t="s">
+        <v>432</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="B114" t="s">
+        <v>433</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="B115" t="s">
+        <v>434</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
         <v>293</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="B116" t="s">
+        <v>337</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="B117" t="s">
+        <v>435</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="B118" t="s">
+        <v>436</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="B119" t="s">
+        <v>437</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="B120" t="s">
+        <v>438</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="B121" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D121" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="B122" t="s">
+        <v>439</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D122" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="B123" t="s">
+        <v>440</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D123" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="B124" t="s">
+        <v>441</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D124" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="B125" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
         <v>294</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="C126" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
         <v>295</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="C127" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
         <v>297</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="C128" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
         <v>298</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="C129" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
         <v>299</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="C130" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D130" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
         <v>296</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="C131" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D131" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="C132" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D132" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
         <v>302</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="C133" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D133" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
         <v>301</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="C134" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D134" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="B136" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="D136" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="B137" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C137" s="7" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="B25" s="13" t="s">
+      <c r="D137" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="B138" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C138" s="7" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="D138" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="B139" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D139" s="7" t="s">
         <v>307</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update current test results.
(lwio: r45045)
</commit_message>
<xml_diff>
--- a/lwio/server/srv/docs/lwio_project.xlsx
+++ b/lwio/server/srv/docs/lwio_project.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="445">
   <si>
     <t>API</t>
   </si>
@@ -1410,6 +1410,12 @@
   </si>
   <si>
     <t>lwiod does support file index</t>
+  </si>
+  <si>
+    <t>Not supported</t>
+  </si>
+  <si>
+    <t>No Stream support yet in lwiod/pvfs.</t>
   </si>
 </sst>
 </file>
@@ -1947,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1957,7 +1963,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1">
@@ -1995,11 +2001,14 @@
       <c r="B3" t="s">
         <v>327</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>317</v>
+      <c r="C3" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2133,8 +2142,8 @@
       <c r="B15" t="s">
         <v>338</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>317</v>
+      <c r="C15" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>317</v>
@@ -2144,8 +2153,8 @@
       <c r="B16" t="s">
         <v>339</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>317</v>
+      <c r="C16" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>317</v>
@@ -2155,8 +2164,8 @@
       <c r="B17" t="s">
         <v>340</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>317</v>
+      <c r="C17" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>317</v>
@@ -2166,8 +2175,8 @@
       <c r="B18" t="s">
         <v>341</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>317</v>
+      <c r="C18" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>317</v>
@@ -2177,8 +2186,8 @@
       <c r="B19" t="s">
         <v>342</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>317</v>
+      <c r="C19" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>317</v>
@@ -2188,8 +2197,8 @@
       <c r="B20" t="s">
         <v>343</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>317</v>
+      <c r="C20" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>317</v>
@@ -2210,8 +2219,8 @@
       <c r="B22" t="s">
         <v>345</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>317</v>
+      <c r="C22" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>317</v>
@@ -2221,8 +2230,8 @@
       <c r="B23" t="s">
         <v>346</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>317</v>
+      <c r="C23" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>317</v>
@@ -2232,8 +2241,8 @@
       <c r="B24" t="s">
         <v>347</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>317</v>
+      <c r="C24" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>317</v>
@@ -2276,8 +2285,8 @@
       <c r="B28" t="s">
         <v>351</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>317</v>
+      <c r="C28" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>317</v>
@@ -2287,8 +2296,8 @@
       <c r="B29" t="s">
         <v>352</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>317</v>
+      <c r="C29" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>317</v>
@@ -2298,8 +2307,8 @@
       <c r="B30" t="s">
         <v>353</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>317</v>
+      <c r="C30" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>317</v>
@@ -2309,8 +2318,8 @@
       <c r="B31" t="s">
         <v>354</v>
       </c>
-      <c r="C31" s="14" t="s">
-        <v>317</v>
+      <c r="C31" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>317</v>
@@ -2320,8 +2329,8 @@
       <c r="B32" t="s">
         <v>355</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>317</v>
+      <c r="C32" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>317</v>
@@ -2331,8 +2340,8 @@
       <c r="B33" t="s">
         <v>356</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>317</v>
+      <c r="C33" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>317</v>
@@ -2342,8 +2351,8 @@
       <c r="B34" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>317</v>
+      <c r="C34" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>317</v>
@@ -2353,8 +2362,8 @@
       <c r="B35" t="s">
         <v>358</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>317</v>
+      <c r="C35" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>317</v>
@@ -2367,8 +2376,8 @@
       <c r="B36" t="s">
         <v>359</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>317</v>
+      <c r="C36" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>317</v>
@@ -2378,8 +2387,8 @@
       <c r="B37" t="s">
         <v>360</v>
       </c>
-      <c r="C37" s="14" t="s">
-        <v>317</v>
+      <c r="C37" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>317</v>
@@ -2389,8 +2398,8 @@
       <c r="B38" t="s">
         <v>361</v>
       </c>
-      <c r="C38" s="14" t="s">
-        <v>317</v>
+      <c r="C38" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>317</v>
@@ -2400,8 +2409,8 @@
       <c r="B39" t="s">
         <v>362</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>317</v>
+      <c r="C39" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>317</v>
@@ -2411,8 +2420,8 @@
       <c r="B40" t="s">
         <v>363</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>317</v>
+      <c r="C40" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>317</v>
@@ -2422,8 +2431,8 @@
       <c r="B41" t="s">
         <v>364</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>317</v>
+      <c r="C41" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>317</v>
@@ -2433,8 +2442,8 @@
       <c r="B42" t="s">
         <v>365</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>317</v>
+      <c r="C42" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>317</v>
@@ -2447,8 +2456,8 @@
       <c r="B43" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>317</v>
+      <c r="C43" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>317</v>
@@ -2458,8 +2467,8 @@
       <c r="B44" t="s">
         <v>367</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>317</v>
+      <c r="C44" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>317</v>
@@ -2469,8 +2478,8 @@
       <c r="B45" t="s">
         <v>337</v>
       </c>
-      <c r="C45" s="14" t="s">
-        <v>317</v>
+      <c r="C45" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>317</v>
@@ -2480,8 +2489,8 @@
       <c r="B46" t="s">
         <v>368</v>
       </c>
-      <c r="C46" s="14" t="s">
-        <v>317</v>
+      <c r="C46" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>317</v>
@@ -2491,8 +2500,8 @@
       <c r="B47" t="s">
         <v>369</v>
       </c>
-      <c r="C47" s="14" t="s">
-        <v>317</v>
+      <c r="C47" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>317</v>
@@ -2502,8 +2511,8 @@
       <c r="B48" t="s">
         <v>370</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>317</v>
+      <c r="C48" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>317</v>
@@ -2513,8 +2522,8 @@
       <c r="B49" t="s">
         <v>371</v>
       </c>
-      <c r="C49" s="14" t="s">
-        <v>317</v>
+      <c r="C49" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D49" s="14" t="s">
         <v>317</v>
@@ -2524,8 +2533,8 @@
       <c r="B50" t="s">
         <v>372</v>
       </c>
-      <c r="C50" s="14" t="s">
-        <v>317</v>
+      <c r="C50" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="D50" s="14" t="s">
         <v>317</v>
@@ -2535,8 +2544,8 @@
       <c r="B51" t="s">
         <v>373</v>
       </c>
-      <c r="C51" s="14" t="s">
-        <v>317</v>
+      <c r="C51" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D51" s="14" t="s">
         <v>317</v>
@@ -2546,8 +2555,8 @@
       <c r="B52" t="s">
         <v>374</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>317</v>
+      <c r="C52" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D52" s="14" t="s">
         <v>317</v>
@@ -2557,8 +2566,8 @@
       <c r="B53" t="s">
         <v>375</v>
       </c>
-      <c r="C53" s="14" t="s">
-        <v>317</v>
+      <c r="C53" s="13" t="s">
+        <v>315</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>317</v>
@@ -2568,8 +2577,8 @@
       <c r="B54" t="s">
         <v>376</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>317</v>
+      <c r="C54" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>317</v>
@@ -2579,19 +2588,19 @@
       <c r="B55" t="s">
         <v>377</v>
       </c>
-      <c r="C55" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>317</v>
+      <c r="C55" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="B56" t="s">
         <v>378</v>
       </c>
-      <c r="C56" s="14" t="s">
-        <v>317</v>
+      <c r="C56" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>317</v>
@@ -2913,8 +2922,8 @@
       <c r="B81" t="s">
         <v>400</v>
       </c>
-      <c r="C81" s="14" t="s">
-        <v>317</v>
+      <c r="C81" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D81" s="14" t="s">
         <v>317</v>
@@ -2924,8 +2933,8 @@
       <c r="B82" t="s">
         <v>401</v>
       </c>
-      <c r="C82" s="14" t="s">
-        <v>317</v>
+      <c r="C82" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D82" s="14" t="s">
         <v>317</v>
@@ -2935,8 +2944,8 @@
       <c r="B83" t="s">
         <v>402</v>
       </c>
-      <c r="C83" s="14" t="s">
-        <v>317</v>
+      <c r="C83" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D83" s="14" t="s">
         <v>317</v>
@@ -2946,8 +2955,8 @@
       <c r="B84" t="s">
         <v>403</v>
       </c>
-      <c r="C84" s="14" t="s">
-        <v>317</v>
+      <c r="C84" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D84" s="14" t="s">
         <v>317</v>
@@ -2957,8 +2966,8 @@
       <c r="B85" t="s">
         <v>404</v>
       </c>
-      <c r="C85" s="14" t="s">
-        <v>317</v>
+      <c r="C85" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D85" s="14" t="s">
         <v>317</v>
@@ -2968,8 +2977,8 @@
       <c r="B86" t="s">
         <v>405</v>
       </c>
-      <c r="C86" s="14" t="s">
-        <v>317</v>
+      <c r="C86" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D86" s="14" t="s">
         <v>317</v>
@@ -2979,8 +2988,8 @@
       <c r="B87" t="s">
         <v>406</v>
       </c>
-      <c r="C87" s="14" t="s">
-        <v>317</v>
+      <c r="C87" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D87" s="14" t="s">
         <v>317</v>
@@ -2990,8 +2999,8 @@
       <c r="B88" t="s">
         <v>407</v>
       </c>
-      <c r="C88" s="14" t="s">
-        <v>317</v>
+      <c r="C88" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D88" s="14" t="s">
         <v>317</v>
@@ -3001,8 +3010,8 @@
       <c r="B89" t="s">
         <v>408</v>
       </c>
-      <c r="C89" s="14" t="s">
-        <v>317</v>
+      <c r="C89" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D89" s="14" t="s">
         <v>317</v>
@@ -3012,8 +3021,8 @@
       <c r="B90" t="s">
         <v>409</v>
       </c>
-      <c r="C90" s="14" t="s">
-        <v>317</v>
+      <c r="C90" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D90" s="14" t="s">
         <v>317</v>
@@ -3023,8 +3032,8 @@
       <c r="B91" t="s">
         <v>410</v>
       </c>
-      <c r="C91" s="14" t="s">
-        <v>317</v>
+      <c r="C91" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D91" s="14" t="s">
         <v>317</v>
@@ -3034,8 +3043,8 @@
       <c r="B92" t="s">
         <v>411</v>
       </c>
-      <c r="C92" s="14" t="s">
-        <v>317</v>
+      <c r="C92" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D92" s="14" t="s">
         <v>317</v>
@@ -3045,8 +3054,8 @@
       <c r="B93" t="s">
         <v>412</v>
       </c>
-      <c r="C93" s="14" t="s">
-        <v>317</v>
+      <c r="C93" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D93" s="14" t="s">
         <v>317</v>
@@ -3056,8 +3065,8 @@
       <c r="B94" t="s">
         <v>413</v>
       </c>
-      <c r="C94" s="14" t="s">
-        <v>317</v>
+      <c r="C94" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D94" s="14" t="s">
         <v>317</v>
@@ -3067,8 +3076,8 @@
       <c r="B95" t="s">
         <v>414</v>
       </c>
-      <c r="C95" s="14" t="s">
-        <v>317</v>
+      <c r="C95" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D95" s="14" t="s">
         <v>317</v>
@@ -3078,8 +3087,8 @@
       <c r="B96" t="s">
         <v>415</v>
       </c>
-      <c r="C96" s="14" t="s">
-        <v>317</v>
+      <c r="C96" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D96" s="14" t="s">
         <v>317</v>
@@ -3089,8 +3098,8 @@
       <c r="B97" t="s">
         <v>416</v>
       </c>
-      <c r="C97" s="14" t="s">
-        <v>317</v>
+      <c r="C97" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D97" s="14" t="s">
         <v>317</v>
@@ -3100,8 +3109,8 @@
       <c r="B98" t="s">
         <v>417</v>
       </c>
-      <c r="C98" s="14" t="s">
-        <v>317</v>
+      <c r="C98" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D98" s="14" t="s">
         <v>317</v>
@@ -3111,8 +3120,8 @@
       <c r="B99" t="s">
         <v>418</v>
       </c>
-      <c r="C99" s="14" t="s">
-        <v>317</v>
+      <c r="C99" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D99" s="14" t="s">
         <v>317</v>
@@ -3122,8 +3131,8 @@
       <c r="B100" t="s">
         <v>419</v>
       </c>
-      <c r="C100" s="14" t="s">
-        <v>317</v>
+      <c r="C100" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D100" s="14" t="s">
         <v>317</v>
@@ -3133,8 +3142,8 @@
       <c r="B101" t="s">
         <v>420</v>
       </c>
-      <c r="C101" s="14" t="s">
-        <v>317</v>
+      <c r="C101" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D101" s="14" t="s">
         <v>317</v>
@@ -3144,8 +3153,8 @@
       <c r="B102" t="s">
         <v>421</v>
       </c>
-      <c r="C102" s="14" t="s">
-        <v>317</v>
+      <c r="C102" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D102" s="14" t="s">
         <v>317</v>
@@ -3155,8 +3164,8 @@
       <c r="B103" t="s">
         <v>422</v>
       </c>
-      <c r="C103" s="14" t="s">
-        <v>317</v>
+      <c r="C103" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>317</v>
@@ -3166,8 +3175,8 @@
       <c r="B104" t="s">
         <v>423</v>
       </c>
-      <c r="C104" s="14" t="s">
-        <v>317</v>
+      <c r="C104" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D104" s="14" t="s">
         <v>317</v>
@@ -3177,8 +3186,8 @@
       <c r="B105" t="s">
         <v>424</v>
       </c>
-      <c r="C105" s="14" t="s">
-        <v>317</v>
+      <c r="C105" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>317</v>
@@ -3188,8 +3197,8 @@
       <c r="B106" t="s">
         <v>425</v>
       </c>
-      <c r="C106" s="14" t="s">
-        <v>317</v>
+      <c r="C106" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D106" s="14" t="s">
         <v>317</v>
@@ -3199,8 +3208,8 @@
       <c r="B107" t="s">
         <v>426</v>
       </c>
-      <c r="C107" s="14" t="s">
-        <v>317</v>
+      <c r="C107" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D107" s="14" t="s">
         <v>317</v>
@@ -3210,8 +3219,8 @@
       <c r="B108" t="s">
         <v>427</v>
       </c>
-      <c r="C108" s="14" t="s">
-        <v>317</v>
+      <c r="C108" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D108" s="14" t="s">
         <v>317</v>
@@ -3221,8 +3230,8 @@
       <c r="B109" t="s">
         <v>428</v>
       </c>
-      <c r="C109" s="14" t="s">
-        <v>317</v>
+      <c r="C109" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D109" s="14" t="s">
         <v>317</v>
@@ -3232,8 +3241,8 @@
       <c r="B110" t="s">
         <v>429</v>
       </c>
-      <c r="C110" s="14" t="s">
-        <v>317</v>
+      <c r="C110" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D110" s="14" t="s">
         <v>317</v>
@@ -3243,8 +3252,8 @@
       <c r="B111" t="s">
         <v>430</v>
       </c>
-      <c r="C111" s="14" t="s">
-        <v>317</v>
+      <c r="C111" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D111" s="14" t="s">
         <v>317</v>
@@ -3254,160 +3263,163 @@
       <c r="B112" t="s">
         <v>431</v>
       </c>
-      <c r="C112" s="14" t="s">
-        <v>317</v>
+      <c r="C112" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D112" s="14" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="B113" t="s">
         <v>432</v>
       </c>
-      <c r="C113" s="14" t="s">
-        <v>317</v>
+      <c r="C113" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D113" s="14" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:5">
       <c r="B114" t="s">
         <v>433</v>
       </c>
-      <c r="C114" s="14" t="s">
-        <v>317</v>
+      <c r="C114" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D114" s="14" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:5">
       <c r="B115" t="s">
         <v>434</v>
       </c>
-      <c r="C115" s="14" t="s">
-        <v>317</v>
+      <c r="C115" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D115" s="14" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>293</v>
       </c>
       <c r="B116" t="s">
         <v>337</v>
       </c>
-      <c r="C116" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="C116" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D116" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E116" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="B117" t="s">
         <v>435</v>
       </c>
-      <c r="C117" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="C117" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="B118" t="s">
         <v>436</v>
       </c>
-      <c r="C118" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="C118" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D118" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="B119" t="s">
         <v>437</v>
       </c>
-      <c r="C119" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="C119" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D119" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="B120" t="s">
         <v>438</v>
       </c>
-      <c r="C120" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D120" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="C120" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D120" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="B121" t="s">
         <v>30</v>
       </c>
-      <c r="C121" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
+      <c r="C121" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="B122" t="s">
         <v>439</v>
       </c>
-      <c r="C122" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D122" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="C122" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D122" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="B123" t="s">
         <v>440</v>
       </c>
-      <c r="C123" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D123" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="C123" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D123" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="B124" t="s">
         <v>441</v>
       </c>
-      <c r="C124" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="C124" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D124" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="B125" t="s">
         <v>29</v>
       </c>
-      <c r="C125" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="C125" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D125" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>294</v>
       </c>
@@ -3418,23 +3430,23 @@
         <v>314</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>295</v>
       </c>
-      <c r="C127" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="C127" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>297</v>
       </c>
-      <c r="C128" s="14" t="s">
-        <v>317</v>
+      <c r="C128" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D128" s="14" t="s">
         <v>317</v>
@@ -3444,8 +3456,8 @@
       <c r="A129" t="s">
         <v>298</v>
       </c>
-      <c r="C129" s="14" t="s">
-        <v>317</v>
+      <c r="C129" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D129" s="14" t="s">
         <v>317</v>
@@ -3455,19 +3467,19 @@
       <c r="A130" t="s">
         <v>299</v>
       </c>
-      <c r="C130" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="D130" s="14" t="s">
-        <v>317</v>
+      <c r="C130" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>296</v>
       </c>
-      <c r="C131" s="14" t="s">
-        <v>317</v>
+      <c r="C131" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D131" s="14" t="s">
         <v>317</v>
@@ -3477,8 +3489,8 @@
       <c r="A132" t="s">
         <v>300</v>
       </c>
-      <c r="C132" s="14" t="s">
-        <v>317</v>
+      <c r="C132" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D132" s="14" t="s">
         <v>317</v>
@@ -3488,8 +3500,8 @@
       <c r="A133" t="s">
         <v>302</v>
       </c>
-      <c r="C133" s="14" t="s">
-        <v>317</v>
+      <c r="C133" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="D133" s="14" t="s">
         <v>317</v>

</xml_diff>